<commit_message>
agregando congresista faltante complice
</commit_message>
<xml_diff>
--- a/infocongresistas.xlsx
+++ b/infocongresistas.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseincio/Documents/muro-verguenza-peru/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D630E277-4A88-5242-A2AC-6840DC57DBD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B9FB69-36E2-5A4C-A031-D324D959C07A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="800" windowWidth="25040" windowHeight="13880" xr2:uid="{D13D0022-5F2B-AB40-9C6A-61466BD4ECD0}"/>
+    <workbookView xWindow="300" yWindow="620" windowWidth="25040" windowHeight="13880" xr2:uid="{D13D0022-5F2B-AB40-9C6A-61466BD4ECD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$131</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1320,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD3970C-88B8-E242-9347-053CDA7858CB}">
   <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2675,6 +2675,9 @@
       </c>
       <c r="H51">
         <v>3</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>